<commit_message>
Updated club table (mostly just testing Slack integration)
</commit_message>
<xml_diff>
--- a/Modified Club Database 2015-2016.xlsx
+++ b/Modified Club Database 2015-2016.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26207"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26311"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chanan/Google Drive/Bellarmine/12th Grade/Web Applications/Club Registration App/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chanan/Google Drive/Developer/Carillon Software Team/clubs-management/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="220" yWindow="520" windowWidth="38260" windowHeight="22580"/>
+    <workbookView xWindow="140" yWindow="520" windowWidth="38260" windowHeight="22580"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="747" uniqueCount="585">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="766" uniqueCount="586">
   <si>
     <t>Name</t>
   </si>
@@ -1779,13 +1779,16 @@
   </si>
   <si>
     <t>Club ID</t>
+  </si>
+  <si>
+    <t>Extra</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1819,6 +1822,12 @@
       <sz val="11"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1840,7 +1849,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1870,6 +1879,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2173,8 +2183,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S1034"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="104" workbookViewId="0">
-      <selection activeCell="D119" sqref="D119"/>
+    <sheetView tabSelected="1" topLeftCell="A102" zoomScale="104" workbookViewId="0">
+      <selection activeCell="A134" sqref="A134:A152"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5990,7 +6000,9 @@
       <c r="H133" s="2"/>
     </row>
     <row r="134" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A134" s="2"/>
+      <c r="A134" s="19" t="s">
+        <v>585</v>
+      </c>
       <c r="B134" s="2"/>
       <c r="C134" s="14">
         <v>324209</v>
@@ -6005,7 +6017,9 @@
       <c r="H134" s="2"/>
     </row>
     <row r="135" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A135" s="2"/>
+      <c r="A135" s="19" t="s">
+        <v>585</v>
+      </c>
       <c r="B135" s="2"/>
       <c r="C135" s="14">
         <v>907273</v>
@@ -6020,7 +6034,9 @@
       <c r="H135" s="2"/>
     </row>
     <row r="136" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A136" s="2"/>
+      <c r="A136" s="19" t="s">
+        <v>585</v>
+      </c>
       <c r="B136" s="2"/>
       <c r="C136" s="14">
         <v>792098</v>
@@ -6035,7 +6051,9 @@
       <c r="H136" s="2"/>
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A137" s="2"/>
+      <c r="A137" s="19" t="s">
+        <v>585</v>
+      </c>
       <c r="B137" s="2"/>
       <c r="C137" s="14">
         <v>523858</v>
@@ -6050,7 +6068,9 @@
       <c r="H137" s="2"/>
     </row>
     <row r="138" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A138" s="2"/>
+      <c r="A138" s="19" t="s">
+        <v>585</v>
+      </c>
       <c r="B138" s="2"/>
       <c r="C138" s="14">
         <v>690546</v>
@@ -6065,7 +6085,9 @@
       <c r="H138" s="2"/>
     </row>
     <row r="139" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A139" s="2"/>
+      <c r="A139" s="19" t="s">
+        <v>585</v>
+      </c>
       <c r="B139" s="2"/>
       <c r="C139" s="14">
         <v>635134</v>
@@ -6080,7 +6102,9 @@
       <c r="H139" s="2"/>
     </row>
     <row r="140" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A140" s="2"/>
+      <c r="A140" s="19" t="s">
+        <v>585</v>
+      </c>
       <c r="B140" s="2"/>
       <c r="C140" s="14">
         <v>300599</v>
@@ -6095,7 +6119,9 @@
       <c r="H140" s="2"/>
     </row>
     <row r="141" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A141" s="2"/>
+      <c r="A141" s="19" t="s">
+        <v>585</v>
+      </c>
       <c r="B141" s="2"/>
       <c r="C141" s="14">
         <v>152476</v>
@@ -6110,7 +6136,9 @@
       <c r="H141" s="2"/>
     </row>
     <row r="142" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A142" s="2"/>
+      <c r="A142" s="19" t="s">
+        <v>585</v>
+      </c>
       <c r="B142" s="2"/>
       <c r="C142" s="14">
         <v>646908</v>
@@ -6125,7 +6153,9 @@
       <c r="H142" s="2"/>
     </row>
     <row r="143" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A143" s="2"/>
+      <c r="A143" s="19" t="s">
+        <v>585</v>
+      </c>
       <c r="B143" s="2"/>
       <c r="C143" s="14">
         <v>433430</v>
@@ -6140,7 +6170,9 @@
       <c r="H143" s="2"/>
     </row>
     <row r="144" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A144" s="2"/>
+      <c r="A144" s="19" t="s">
+        <v>585</v>
+      </c>
       <c r="B144" s="2"/>
       <c r="C144" s="14">
         <v>800953</v>
@@ -6155,7 +6187,9 @@
       <c r="H144" s="2"/>
     </row>
     <row r="145" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A145" s="2"/>
+      <c r="A145" s="19" t="s">
+        <v>585</v>
+      </c>
       <c r="B145" s="2"/>
       <c r="C145" s="14">
         <v>302861</v>
@@ -6170,7 +6204,9 @@
       <c r="H145" s="2"/>
     </row>
     <row r="146" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A146" s="2"/>
+      <c r="A146" s="19" t="s">
+        <v>585</v>
+      </c>
       <c r="B146" s="2"/>
       <c r="C146" s="14">
         <v>672591</v>
@@ -6185,7 +6221,9 @@
       <c r="H146" s="2"/>
     </row>
     <row r="147" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A147" s="2"/>
+      <c r="A147" s="19" t="s">
+        <v>585</v>
+      </c>
       <c r="B147" s="2"/>
       <c r="C147" s="14">
         <v>297537</v>
@@ -6200,7 +6238,9 @@
       <c r="H147" s="2"/>
     </row>
     <row r="148" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A148" s="2"/>
+      <c r="A148" s="19" t="s">
+        <v>585</v>
+      </c>
       <c r="B148" s="2"/>
       <c r="C148" s="14">
         <v>439551</v>
@@ -6215,7 +6255,9 @@
       <c r="H148" s="2"/>
     </row>
     <row r="149" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A149" s="2"/>
+      <c r="A149" s="19" t="s">
+        <v>585</v>
+      </c>
       <c r="B149" s="2"/>
       <c r="C149" s="14">
         <v>985804</v>
@@ -6230,7 +6272,9 @@
       <c r="H149" s="2"/>
     </row>
     <row r="150" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A150" s="2"/>
+      <c r="A150" s="19" t="s">
+        <v>585</v>
+      </c>
       <c r="B150" s="2"/>
       <c r="C150" s="14">
         <v>924624</v>
@@ -6245,7 +6289,9 @@
       <c r="H150" s="2"/>
     </row>
     <row r="151" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A151" s="2"/>
+      <c r="A151" s="19" t="s">
+        <v>585</v>
+      </c>
       <c r="B151" s="2"/>
       <c r="C151" s="14">
         <v>650702</v>
@@ -6260,7 +6306,9 @@
       <c r="H151" s="2"/>
     </row>
     <row r="152" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A152" s="2"/>
+      <c r="A152" s="19" t="s">
+        <v>585</v>
+      </c>
       <c r="B152" s="2"/>
       <c r="C152" s="14">
         <v>252077</v>

</xml_diff>